<commit_message>
learning w/o ordinal encoder
</commit_message>
<xml_diff>
--- a/BDS/variables.xlsx
+++ b/BDS/variables.xlsx
@@ -31,10 +31,10 @@
     <t>aveVelocity</t>
   </si>
   <si>
-    <t>MVPA_minutes.week</t>
+    <t>MVPA</t>
   </si>
   <si>
-    <t>IPAQ_Category</t>
+    <t>IPAQ</t>
   </si>
   <si>
     <t>Subject</t>

</xml_diff>